<commit_message>
Annotated clusters, next step is subclustering
</commit_message>
<xml_diff>
--- a/Metadata/cluster_annotation_map.xlsx
+++ b/Metadata/cluster_annotation_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiquepaul/xRobinson Group/01_Systemic Sclerosis/Metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiquepaul/xRobinson Group/02_Protocol/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26946465-5A5A-1547-ADF1-25C73F6B166D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6454092-D515-9B48-B363-105AE04A4082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fresh_v_control" sheetId="1" r:id="rId1"/>
@@ -20,28 +20,19 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Colors!$G$1:$H$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fresh_v_control!$A$1:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fresh_v_control!$A$1:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="45">
   <si>
     <t>Cluster ID</t>
   </si>
@@ -103,12 +94,6 @@
     <t>Integrated dataset, k=24</t>
   </si>
   <si>
-    <t>Integrated dataset, k=25</t>
-  </si>
-  <si>
-    <t>Integrated dataset, k=26</t>
-  </si>
-  <si>
     <t>Melanocytes/Schwann cells/Neuronal cells</t>
   </si>
   <si>
@@ -124,15 +109,6 @@
     <t>Integrated dataset, k=30</t>
   </si>
   <si>
-    <t>Integrated dataset, k=31</t>
-  </si>
-  <si>
-    <t>Integrated dataset, k=32</t>
-  </si>
-  <si>
-    <t>add manual</t>
-  </si>
-  <si>
     <t>Melanocytes/Schwann cells</t>
   </si>
   <si>
@@ -188,6 +164,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>fresh/cultured combined (n=6)</t>
   </si>
 </sst>
 </file>
@@ -241,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -251,9 +230,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,6 +241,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,16 +527,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,211 +559,178 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
-        <v>6</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
-        <v>8</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
-        <v>14</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
-        <v>11</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="2">
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
-        <v>19</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
-        <v>5</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C16" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
-      <sortCondition ref="B1:B20"/>
+  <autoFilter ref="A1:C14" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
+      <sortCondition ref="B1:B17"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -790,15 +739,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B446C118-5282-2C4F-B30F-0DD13B148AA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="28.1640625" customWidth="1"/>
   </cols>
@@ -819,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -841,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -869,8 +819,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -882,7 +832,7 @@
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -893,7 +843,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -915,10 +865,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -930,17 +880,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FA805A-61FF-0840-9131-82DB7F4A8505}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="8" max="9" width="21.83203125" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" customWidth="1"/>
@@ -958,156 +908,178 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
+      <c r="A2" s="10">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A3" s="10">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="11">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="11">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="11">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="11">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="6">
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="11">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A15" s="10">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="6">
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A16" s="10">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="C17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1115,14 +1087,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DACD5DA-A5A4-8F42-9F0D-16A2F617EF4C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -1130,238 +1102,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="G1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>48</v>
+      <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H2">
         <v>0.26621364624329147</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>0.28647562100512458</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="H4">
         <v>0.31307070750923216</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H5">
         <v>0.3453043555518005</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="9"/>
+      <c r="D6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="8"/>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H6">
         <v>0.39910665459517825</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="9"/>
+      <c r="D7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="8"/>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H7">
         <v>0.5413970734982384</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="A8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9"/>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H8">
         <v>0.62381063491692834</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="H9">
         <v>0.64373967130605225</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H10">
         <v>0.66073417852183269</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H11">
         <v>0.7501108716967404</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
+      <c r="A12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H12">
         <v>0.80062948265946876</v>
@@ -1369,16 +1341,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:H12" xr:uid="{1DACD5DA-A5A4-8F42-9F0D-16A2F617EF4C}">
+  <autoFilter ref="G1:H12" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:H12">
       <sortCondition ref="H1:H12"/>
     </sortState>

</xml_diff>

<commit_message>
Subclustering of fresh samples
</commit_message>
<xml_diff>
--- a/Metadata/cluster_annotation_map.xlsx
+++ b/Metadata/cluster_annotation_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiquepaul/xRobinson Group/02_Protocol/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6454092-D515-9B48-B363-105AE04A4082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05BB0B2-D596-0A4C-B6F5-83F3D395CDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fresh_v_control" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -246,6 +246,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -552,175 +559,175 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="A2" s="12">
+        <v>8</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="14">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="14">
+        <v>6</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A5" s="12">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A6" s="12">
+        <v>7</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A7" s="12">
+        <v>10</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A8" s="12">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A9" s="12">
+        <v>12</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A10" s="12">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="14">
+        <v>16</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A12" s="12">
+        <v>15</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A14" s="12">
+        <v>14</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="14">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+      <c r="B15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="14">
+        <v>9</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
+      <c r="A17" s="14">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
@@ -742,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>